<commit_message>
future enhancements for user-stories in tts_ui
</commit_message>
<xml_diff>
--- a/Plans/TTS_UI (1).xlsx
+++ b/Plans/TTS_UI (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6232e5fddcee7410/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6232e5fddcee7410/Desktop/FinSight/Plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{517277F4-C5FB-43EF-A058-E33C413D2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0739E71-DBAC-434C-AA7C-63E6B1E39DEF}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{517277F4-C5FB-43EF-A058-E33C413D2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69A2C131-1B4D-4910-B88D-C88450C49CE3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Sl No</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t>Scroll bar is out of the div</t>
+  </si>
+  <si>
+    <t>Future Enhancements</t>
   </si>
 </sst>
 </file>
@@ -882,6 +885,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1171,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,10 +1192,11 @@
     <col min="5" max="5" width="39.44140625" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="27.21875" customWidth="1"/>
+    <col min="8" max="8" width="39.88671875" customWidth="1"/>
+    <col min="9" max="9" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1213,8 +1221,11 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1239,8 +1250,9 @@
       <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1265,8 +1277,9 @@
       <c r="H3" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1291,8 +1304,9 @@
       <c r="H4" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1317,8 +1331,9 @@
       <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1343,8 +1358,9 @@
       <c r="H6" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1369,8 +1385,9 @@
       <c r="H7" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1395,8 +1412,9 @@
       <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1421,6 +1439,7 @@
       <c r="H9" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="I9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1431,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEADA1C-1897-441F-992C-D46F8E573E89}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TTS Plan transaction table
</commit_message>
<xml_diff>
--- a/Plans/TTS_UI (1).xlsx
+++ b/Plans/TTS_UI (1).xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6232e5fddcee7410/Desktop/FinSight/Plans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{517277F4-C5FB-43EF-A058-E33C413D2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69A2C131-1B4D-4910-B88D-C88450C49CE3}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{517277F4-C5FB-43EF-A058-E33C413D2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4522F724-3DD4-45B8-AA62-AB2AB4F180BA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Defects" sheetId="2" r:id="rId2"/>
+    <sheet name="transaction table" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Sl No</t>
   </si>
@@ -592,12 +593,81 @@
   <si>
     <t>Future Enhancements</t>
   </si>
+  <si>
+    <t>refer sheet-3</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Recepeint</t>
+  </si>
+  <si>
+    <t>transaction type</t>
+  </si>
+  <si>
+    <t>vendor app</t>
+  </si>
+  <si>
+    <t>transaction number</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>modify</t>
+  </si>
+  <si>
+    <t>15/01/2026  12:24:00 PM IST</t>
+  </si>
+  <si>
+    <t>Amount (Rupees)</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>PayTM</t>
+  </si>
+  <si>
+    <t>txn123009800000645</t>
+  </si>
+  <si>
+    <t>Mechanical chair</t>
+  </si>
+  <si>
+    <t>from date - to date filter</t>
+  </si>
+  <si>
+    <t>date, from time - to time filter</t>
+  </si>
+  <si>
+    <t>from - to amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dropdown for </t>
+  </si>
+  <si>
+    <t>all apps</t>
+  </si>
+  <si>
+    <t>textbox and search icon</t>
+  </si>
+  <si>
+    <t>text box and search icon</t>
+  </si>
+  <si>
+    <t>credit and debit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +687,21 @@
       <i/>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -823,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -870,6 +955,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,7 +1429,9 @@
       <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -1536,4 +1636,176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310137A8-0EC2-41C2-B79E-CDA680ADAB28}">
+  <dimension ref="B5:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="16"/>
+    <col min="2" max="2" width="25.5546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="20" style="16" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="14" style="16" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="24">
+        <v>5000</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>